<commit_message>
work on port table
</commit_message>
<xml_diff>
--- a/Hardware/uC_Port_Table.xlsx
+++ b/Hardware/uC_Port_Table.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Documents\19_git\Reflow\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E422E23C-A60F-4F06-B75A-1BC3AAE42A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329F1A02-4860-4008-86C4-F6B399869C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="LQFP32" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LQFP32!$A$1:$I$26</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="68">
   <si>
     <t>#</t>
   </si>
@@ -214,6 +217,21 @@
   </si>
   <si>
     <t>~INT_EMERGENCY_STOP</t>
+  </si>
+  <si>
+    <t>EXTI0</t>
+  </si>
+  <si>
+    <t>EXTI1</t>
+  </si>
+  <si>
+    <t>trigger on falling edge</t>
+  </si>
+  <si>
+    <t>EXTI2</t>
+  </si>
+  <si>
+    <t>input for emergency stop interrup ttrigger</t>
   </si>
 </sst>
 </file>
@@ -540,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,6 +872,12 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
       <c r="E12" t="s">
         <v>45</v>
       </c>
@@ -871,6 +895,12 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
       <c r="E13" t="s">
         <v>46</v>
       </c>
@@ -888,6 +918,12 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
       <c r="E14" t="s">
         <v>47</v>
       </c>
@@ -905,6 +941,12 @@
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
       <c r="E15" t="s">
         <v>50</v>
       </c>
@@ -925,6 +967,12 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
       <c r="E16" t="s">
         <v>51</v>
       </c>
@@ -945,6 +993,12 @@
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
       <c r="E17" t="s">
         <v>52</v>
       </c>
@@ -964,6 +1018,12 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
       </c>
       <c r="E18" t="s">
         <v>53</v>
@@ -985,6 +1045,15 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
       <c r="E19" t="s">
         <v>57</v>
       </c>
@@ -996,12 +1065,24 @@
       </c>
       <c r="H19" t="s">
         <v>17</v>
+      </c>
+      <c r="I19" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
       <c r="E20" t="s">
         <v>60</v>
       </c>
@@ -1013,63 +1094,42 @@
       </c>
       <c r="H20" t="s">
         <v>17</v>
+      </c>
+      <c r="I20" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
       <c r="E21" t="s">
         <v>62</v>
       </c>
       <c r="F21" t="s">
         <v>40</v>
       </c>
+      <c r="G21" t="s">
+        <v>67</v>
+      </c>
       <c r="H21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="H22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="H23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="H24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="H25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="H26" t="s">
-        <v>17</v>
+      <c r="I21" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I26" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
changed port table + updated schema
</commit_message>
<xml_diff>
--- a/Hardware/uC_Port_Table.xlsx
+++ b/Hardware/uC_Port_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Documents\19_git\Reflow\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329F1A02-4860-4008-86C4-F6B399869C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95408F2-EC1B-4246-81BC-45542906AE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="LQFP32" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LQFP32!$A$1:$I$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LQFP32!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
   <si>
     <t>#</t>
   </si>
@@ -180,27 +180,9 @@
     <t>Function description</t>
   </si>
   <si>
-    <t>HSS_1_EN</t>
-  </si>
-  <si>
-    <t>HSS_2_EN</t>
-  </si>
-  <si>
-    <t>HSS_3_EN</t>
-  </si>
-  <si>
-    <t>HSS_4_EN</t>
-  </si>
-  <si>
     <t>IO</t>
   </si>
   <si>
-    <t>Aux high side switch power output</t>
-  </si>
-  <si>
-    <t>AUX</t>
-  </si>
-  <si>
     <t>~TEMP_DATA_READY</t>
   </si>
   <si>
@@ -232,6 +214,9 @@
   </si>
   <si>
     <t>input for emergency stop interrup ttrigger</t>
+  </si>
+  <si>
+    <t>GPIO</t>
   </si>
 </sst>
 </file>
@@ -558,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +734,7 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
@@ -775,7 +760,7 @@
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
@@ -878,6 +863,9 @@
       <c r="C12">
         <v>7</v>
       </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
       <c r="E12" t="s">
         <v>45</v>
       </c>
@@ -901,6 +889,9 @@
       <c r="C13">
         <v>6</v>
       </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
       <c r="E13" t="s">
         <v>46</v>
       </c>
@@ -924,6 +915,9 @@
       <c r="C14">
         <v>12</v>
       </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
       <c r="E14" t="s">
         <v>47</v>
       </c>
@@ -939,45 +933,51 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G16" t="s">
         <v>55</v>
@@ -986,150 +986,40 @@
         <v>17</v>
       </c>
       <c r="I16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="H17" t="s">
         <v>17</v>
       </c>
       <c r="I17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" t="s">
         <v>59</v>
       </c>
-      <c r="H19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" t="s">
-        <v>65</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I26" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I22" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
work on porttable and on layout of temperature sensor
</commit_message>
<xml_diff>
--- a/Hardware/uC_Port_Table.xlsx
+++ b/Hardware/uC_Port_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Documents\19_git\Reflow\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95408F2-EC1B-4246-81BC-45542906AE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FBCCF9-054B-4119-819F-59A4DBC202C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
   <si>
     <t>#</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>GPIO</t>
+  </si>
+  <si>
+    <t>~CS_TEMP</t>
+  </si>
+  <si>
+    <t>Temperature SPI chipselect</t>
   </si>
 </sst>
 </file>
@@ -543,22 +549,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -587,7 +593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -613,7 +619,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -639,7 +645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -665,7 +671,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -691,7 +697,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -717,7 +723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -743,7 +749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -769,7 +775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -798,7 +804,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -827,7 +833,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -853,7 +859,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -879,7 +885,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -905,7 +911,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -931,7 +937,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>18</v>
       </c>
@@ -960,7 +966,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>19</v>
       </c>
@@ -989,7 +995,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>20</v>
       </c>
@@ -1016,6 +1022,32 @@
       </c>
       <c r="I17" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>